<commit_message>
wrap up limma and deseq functions
</commit_message>
<xml_diff>
--- a/auto_examples_jupyter/limma_output.xlsx
+++ b/auto_examples_jupyter/limma_output.xlsx
@@ -397,76 +397,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>gene5</t>
+          <t>gene1</t>
         </is>
       </c>
       <c r="B2">
-        <v>-20.28571428571429</v>
+        <v>-1.17938635672426</v>
       </c>
       <c r="C2">
-        <v>20.8</v>
+        <v>14.22088115326463</v>
       </c>
       <c r="D2">
-        <v>-4.524534316254403</v>
+        <v>-4.205265466015536</v>
       </c>
       <c r="E2">
-        <v>0.001214463125847199</v>
+        <v>2.8465026707544e-05</v>
       </c>
       <c r="F2">
-        <v>0.01214463125847199</v>
+        <v>0.00028465026707544</v>
       </c>
       <c r="G2">
-        <v>-3.222684512418237</v>
+        <v>2.189932207218739</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>gene10</t>
+          <t>gene5</t>
         </is>
       </c>
       <c r="B3">
-        <v>-6.285714285714288</v>
+        <v>-0.6324493433217881</v>
       </c>
       <c r="C3">
-        <v>7.6</v>
+        <v>16.3443560659832</v>
       </c>
       <c r="D3">
-        <v>-1.977736073394964</v>
+        <v>-3.70888153777021</v>
       </c>
       <c r="E3">
-        <v>0.07729663318759673</v>
+        <v>0.0002198669051132755</v>
       </c>
       <c r="F3">
-        <v>0.3864831659379837</v>
+        <v>0.001099334525566378</v>
       </c>
       <c r="G3">
-        <v>-4.211041225005055</v>
+        <v>-0.102360119616943</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gene9</t>
+          <t>gene4</t>
         </is>
       </c>
       <c r="B4">
-        <v>10.95238095238094</v>
+        <v>0.3639954574941058</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>18.3113081730598</v>
       </c>
       <c r="D4">
-        <v>1.634712004931864</v>
+        <v>3.174407221009857</v>
       </c>
       <c r="E4">
-        <v>0.1343652912677906</v>
+        <v>0.001548245361016576</v>
       </c>
       <c r="F4">
-        <v>0.4478843042259689</v>
+        <v>0.005160817870055252</v>
       </c>
       <c r="G4">
-        <v>-4.373728365528439</v>
+        <v>-2.29158336899609</v>
       </c>
     </row>
     <row r="5">
@@ -476,22 +476,22 @@
         </is>
       </c>
       <c r="B5">
-        <v>9.19047619047619</v>
+        <v>-0.5663683886699804</v>
       </c>
       <c r="C5">
-        <v>16.1</v>
+        <v>16.02534944916673</v>
       </c>
       <c r="D5">
-        <v>1.284444293067966</v>
+        <v>-3.074341718212893</v>
       </c>
       <c r="E5">
-        <v>0.2290585879443582</v>
+        <v>0.002168084464122608</v>
       </c>
       <c r="F5">
-        <v>0.4721948280578002</v>
+        <v>0.005420211160306521</v>
       </c>
       <c r="G5">
-        <v>-4.53014103437416</v>
+        <v>-2.164716618960036</v>
       </c>
     </row>
     <row r="6">
@@ -501,147 +501,147 @@
         </is>
       </c>
       <c r="B6">
-        <v>4.571428571428572</v>
+        <v>0.5584724117960018</v>
       </c>
       <c r="C6">
-        <v>7.2</v>
+        <v>13.58519099544315</v>
       </c>
       <c r="D6">
-        <v>1.263723450617177</v>
+        <v>1.911613288845917</v>
       </c>
       <c r="E6">
-        <v>0.2360974140289001</v>
+        <v>0.05621723165508651</v>
       </c>
       <c r="F6">
-        <v>0.4721948280578002</v>
+        <v>0.112434463310173</v>
       </c>
       <c r="G6">
-        <v>-4.538856141805008</v>
+        <v>-4.608396723735679</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>gene1</t>
+          <t>gene8</t>
         </is>
       </c>
       <c r="B7">
-        <v>-2.761904761904761</v>
+        <v>0.2351166788199528</v>
       </c>
       <c r="C7">
-        <v>4.4</v>
+        <v>16.97684981952542</v>
       </c>
       <c r="D7">
-        <v>-0.6261591596541626</v>
+        <v>1.613410667212506</v>
       </c>
       <c r="E7">
-        <v>0.54578171212534</v>
+        <v>0.1069772502976971</v>
       </c>
       <c r="F7">
-        <v>0.8211362494373966</v>
+        <v>0.1782954171628285</v>
       </c>
       <c r="G7">
-        <v>-4.757958331631413</v>
+        <v>-5.777154420298248</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>gene4</t>
+          <t>gene9</t>
         </is>
       </c>
       <c r="B8">
-        <v>15.61904761904759</v>
+        <v>0.1561028444463624</v>
       </c>
       <c r="C8">
-        <v>108.6</v>
+        <v>16.8669522266167</v>
       </c>
       <c r="D8">
-        <v>0.4699617810953804</v>
+        <v>1.043096188344876</v>
       </c>
       <c r="E8">
-        <v>0.6488558385485885</v>
+        <v>0.2971609858261296</v>
       </c>
       <c r="F8">
-        <v>0.8211362494373966</v>
+        <v>0.3943164205625868</v>
       </c>
       <c r="G8">
-        <v>-4.792609902756064</v>
+        <v>-6.503116479686732</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>gene6</t>
+          <t>gene7</t>
         </is>
       </c>
       <c r="B9">
-        <v>1.571428571428569</v>
+        <v>-0.1658160195647369</v>
       </c>
       <c r="C9">
-        <v>5.1</v>
+        <v>16.4440834168446</v>
       </c>
       <c r="D9">
-        <v>0.3538698246051475</v>
+        <v>-1.004359804931692</v>
       </c>
       <c r="E9">
-        <v>0.7310701354339229</v>
+        <v>0.3154531364500694</v>
       </c>
       <c r="F9">
-        <v>0.8211362494373966</v>
+        <v>0.3943164205625868</v>
       </c>
       <c r="G9">
-        <v>-4.812395054140928</v>
+        <v>-6.445890375171244</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>gene8</t>
+          <t>gene10</t>
         </is>
       </c>
       <c r="B10">
-        <v>3.19047619047619</v>
+        <v>-0.235124282266133</v>
       </c>
       <c r="C10">
-        <v>38.9</v>
+        <v>14.83914834046315</v>
       </c>
       <c r="D10">
-        <v>0.2392457028622706</v>
+        <v>-0.8968133847476746</v>
       </c>
       <c r="E10">
-        <v>0.8159355870224907</v>
+        <v>0.370038751762738</v>
       </c>
       <c r="F10">
-        <v>0.8211362494373966</v>
+        <v>0.4111541686252645</v>
       </c>
       <c r="G10">
-        <v>-4.826651288334152</v>
+        <v>-6.097000591079622</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>gene7</t>
+          <t>gene6</t>
         </is>
       </c>
       <c r="B11">
-        <v>2.476190476190471</v>
+        <v>-0.02286980402421968</v>
       </c>
       <c r="C11">
-        <v>33.4</v>
+        <v>13.61861869798013</v>
       </c>
       <c r="D11">
-        <v>0.2323484265761249</v>
+        <v>-0.07805199423126882</v>
       </c>
       <c r="E11">
-        <v>0.8211362494373966</v>
+        <v>0.9378026266757549</v>
       </c>
       <c r="F11">
-        <v>0.8211362494373966</v>
+        <v>0.9378026266757549</v>
       </c>
       <c r="G11">
-        <v>-4.827337426158412</v>
+        <v>-6.378719327334932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>